<commit_message>
Prompt that returns code only (DeepRL)
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatty\Desktop\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tan weijin\Desktop\FYP_sonarcube\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE03C2D0-0B12-469B-87C6-5953E6D038BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252C402B-B2D0-4D3C-9EFC-A93061BB40A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>DeepRL</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Scrapy</t>
+  </si>
+  <si>
+    <t>Code_Only(DeepRL)</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +446,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Heavy Spelling Mistakes prompt
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tan weijin\Desktop\FYP_sonarcube\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252C402B-B2D0-4D3C-9EFC-A93061BB40A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C50E34B-344B-48D8-A648-548A8C5F6808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>DeepRL</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Code_Only(DeepRL)</t>
+  </si>
+  <si>
+    <t>Heavy_Spelling(DeepRL)</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +454,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added dataset into repo list
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tan weijin\Desktop\FYP_sonarcube\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147AD205-97B5-482D-9B5C-3C16E215119D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BCB188-3322-42AB-B156-473463AE5623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>DeepRL</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>only_code_smell(DeepRL)</t>
+  </si>
+  <si>
+    <t>Flowise</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,6 +502,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added refactored datasets for ChatVRM
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BCB188-3322-42AB-B156-473463AE5623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037E9DE0-63EA-425C-B7F9-3B76E1F2A31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>DeepRL</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Flowise</t>
+  </si>
+  <si>
+    <t>ChatVRM</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,6 +510,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated entry to include ChatVRM dataset
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatty\Desktop\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21553B69-6026-4E66-904C-CC2BFB716246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA34CD11-0F93-4D11-8FFF-CE2D3A6BC264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>DeepRL</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>image_super_resolution</t>
+  </si>
+  <si>
+    <t>ChatVRM</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +518,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated entry to include Flowise dataset
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatty\Desktop\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21553B69-6026-4E66-904C-CC2BFB716246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05626D2-AD29-4DB2-8322-7F7F30B258B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="15750" yWindow="2040" windowWidth="7770" windowHeight="13155" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>DeepRL</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>image_super_resolution</t>
+  </si>
+  <si>
+    <t>Flowise</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +518,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed line to prevent merge conflict
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA34CD11-0F93-4D11-8FFF-CE2D3A6BC264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44510299-D6DA-4EB3-BD83-BBAA84F1ED21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="15750" yWindow="2040" windowWidth="7770" windowHeight="13155" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,8 +518,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added flowise dataset into repo.xlsx
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44510299-D6DA-4EB3-BD83-BBAA84F1ED21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10915042-91AC-4E9D-A469-DF83611684B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15750" yWindow="2040" windowWidth="7770" windowHeight="13155" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>DeepRL</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>ChatVRM</t>
+  </si>
+  <si>
+    <t>Flowise</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,6 +521,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Added evaluation of Umami dataset
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14ED41D2-F88D-4DD4-96ED-0135851364A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE0E8A1-26D9-4AD6-9D94-5231AA07A7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15750" yWindow="2040" windowWidth="7770" windowHeight="13155" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>DeepRL</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>ChatVRM</t>
+  </si>
+  <si>
+    <t>Umami</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,6 +534,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added evaluated React Native dataset
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE0E8A1-26D9-4AD6-9D94-5231AA07A7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBA5210-ADB1-4A53-9F96-3860EC9ADC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15750" yWindow="2040" windowWidth="7770" windowHeight="13155" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>DeepRL</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Umami</t>
+  </si>
+  <si>
+    <t>ElasticSearch</t>
+  </si>
+  <si>
+    <t>ReactNative</t>
   </si>
 </sst>
 </file>
@@ -441,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,6 +545,16 @@
         <v>17</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added evaluated SmartTube dataset
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBA5210-ADB1-4A53-9F96-3860EC9ADC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0956456-B705-46DB-BBBA-16CFC4F4B72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>DeepRL</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>ReactNative</t>
+  </si>
+  <si>
+    <t>SmartTube</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
@@ -555,6 +558,11 @@
         <v>19</v>
       </c>
     </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added QuixBugs Java dataset
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0956456-B705-46DB-BBBA-16CFC4F4B72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE9021C-FAA4-414A-9BB0-D39787E09D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>DeepRL</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>SmartTube</t>
+  </si>
+  <si>
+    <t>QuixBugs(Java)</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +566,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added refactored js algorithms dataset
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7E519F-D5AD-498F-9D82-FA79858B28A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E093C042-409A-4281-A104-A28870F442E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1260" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>DeepRL</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>javascript-algorithms-2</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,6 +591,11 @@
         <v>22</v>
       </c>
     </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Merge branch 'correctness-testing' of https://github.com/Winson-Foo/Empirical_Evaluation_of_Commercial_Code_Generation_Models into correctness-testing"
This reverts commit dddfd9645747460bfebc707d76f07137c553774e, reversing
changes made to faed0adc228ee1e0eb850b4296800b37584dd656.
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tan weijin\Desktop\FYP_sonarcube\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E093C042-409A-4281-A104-A28870F442E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147AD205-97B5-482D-9B5C-3C16E215119D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1260" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>DeepRL</t>
   </si>
@@ -75,42 +75,6 @@
   </si>
   <si>
     <t>only_code_smell(DeepRL)</t>
-  </si>
-  <si>
-    <t>PyShortTextCategorization</t>
-  </si>
-  <si>
-    <t>image_super_resolution</t>
-  </si>
-  <si>
-    <t>Flowise</t>
-  </si>
-  <si>
-    <t>ChatVRM</t>
-  </si>
-  <si>
-    <t>Umami</t>
-  </si>
-  <si>
-    <t>ElasticSearch</t>
-  </si>
-  <si>
-    <t>ReactNative</t>
-  </si>
-  <si>
-    <t>SmartTube</t>
-  </si>
-  <si>
-    <t>QuixBugs(Java)</t>
-  </si>
-  <si>
-    <t>javascript-algorithms</t>
-  </si>
-  <si>
-    <t>`</t>
-  </si>
-  <si>
-    <t>javascript-algorithms-2</t>
   </si>
 </sst>
 </file>
@@ -462,138 +426,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'correctness-testing' of https://github.com/Winson-Foo/Empirical_Evaluation_of_Commercial_Code_Generation_Models into correctness-testing""
This reverts commit f900fdeac04dc3e8cbc1b9552bed69dd37d5a306.
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tan weijin\Desktop\FYP_sonarcube\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147AD205-97B5-482D-9B5C-3C16E215119D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E093C042-409A-4281-A104-A28870F442E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="28680" yWindow="-1260" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>DeepRL</t>
   </si>
@@ -75,6 +75,42 @@
   </si>
   <si>
     <t>only_code_smell(DeepRL)</t>
+  </si>
+  <si>
+    <t>PyShortTextCategorization</t>
+  </si>
+  <si>
+    <t>image_super_resolution</t>
+  </si>
+  <si>
+    <t>Flowise</t>
+  </si>
+  <si>
+    <t>ChatVRM</t>
+  </si>
+  <si>
+    <t>Umami</t>
+  </si>
+  <si>
+    <t>ElasticSearch</t>
+  </si>
+  <si>
+    <t>ReactNative</t>
+  </si>
+  <si>
+    <t>SmartTube</t>
+  </si>
+  <si>
+    <t>QuixBugs(Java)</t>
+  </si>
+  <si>
+    <t>javascript-algorithms</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>javascript-algorithms-2</t>
   </si>
 </sst>
 </file>
@@ -426,77 +462,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added QuixBugs corrected java dataset to repo file
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E093C042-409A-4281-A104-A28870F442E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF35376-9D70-47E3-9A9A-695E60A46D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1260" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>DeepRL</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>javascript-algorithms-2</t>
+  </si>
+  <si>
+    <t>QuixBugs(Java_Corrected)</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,6 +599,11 @@
         <v>24</v>
       </c>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update the repo data
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylv3r\Documents\FIT4701\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatty\Desktop\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF35376-9D70-47E3-9A9A-695E60A46D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F828FC1-3689-4B03-AAF0-1E359C7D380B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>DeepRL</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>SmartTube</t>
-  </si>
-  <si>
-    <t>QuixBugs(Java)</t>
   </si>
   <si>
     <t>javascript-algorithms</t>
@@ -465,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +548,7 @@
         <v>14</v>
       </c>
       <c r="M15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -591,17 +588,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove some java project and fix name spelling
</commit_message>
<xml_diff>
--- a/repo.xlsx
+++ b/repo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatty\Desktop\Empirical_Evaluation_of_Commercial_Code_Generation_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F828FC1-3689-4B03-AAF0-1E359C7D380B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043BE405-DC4C-4D06-BC0C-313106E7CD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{A6AD6C32-A3A6-4A3E-B7AF-F1FC55585EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>DeepRL</t>
   </si>
@@ -92,25 +92,16 @@
     <t>Umami</t>
   </si>
   <si>
-    <t>ElasticSearch</t>
-  </si>
-  <si>
-    <t>ReactNative</t>
-  </si>
-  <si>
-    <t>SmartTube</t>
-  </si>
-  <si>
     <t>javascript-algorithms</t>
   </si>
   <si>
     <t>`</t>
   </si>
   <si>
-    <t>javascript-algorithms-2</t>
-  </si>
-  <si>
     <t>QuixBugs(Java_Corrected)</t>
+  </si>
+  <si>
+    <t>javascript_algorithms_2</t>
   </si>
 </sst>
 </file>
@@ -462,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7409778-19EE-4256-8B18-F28E930BD331}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +539,7 @@
         <v>14</v>
       </c>
       <c r="M15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -573,27 +564,12 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>